<commit_message>
added other case study results as well
</commit_message>
<xml_diff>
--- a/Trace Link Prediction/Prediction Task.xlsx
+++ b/Trace Link Prediction/Prediction Task.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvhi\Desktop\MasterThesis\chatgpt\Survey\ChatGPT Responses\Trace Link Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvhi\Desktop\MasterThesis\CaseStudyonChatGPTforRE\Trace Link Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851D1F16-9E21-4CDB-BC51-E500FFD97348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB787B8F-40B5-445F-8253-AF8EF3DAC06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="8" xr2:uid="{5C1440EF-CC57-4B48-BC83-FD0BF2F151DD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="8" xr2:uid="{5C1440EF-CC57-4B48-BC83-FD0BF2F151DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -7684,16 +7684,16 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <f>AVERAGE('Run#1'!J29, 'Run#2'!J29, 'Run#3'!J29, 'Run#4'!J29, 'Run#5'!J29,'Run#6'!J29)</f>
+        <f>AVERAGE('Run#0'!J29,'Run#1'!J29, 'Run#2'!J29, 'Run#3'!J29, 'Run#4'!J29, 'Run#5'!J29,'Run#6'!J29)</f>
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <f>AVERAGE('Run#1'!K29, 'Run#2'!K29, 'Run#3'!K29, 'Run#4'!K29, 'Run#5'!K29,'Run#6'!K29)</f>
-        <v>0.96045259088737367</v>
+        <f>AVERAGE('Run#0'!K29,'Run#1'!K29, 'Run#2'!K29, 'Run#3'!K29, 'Run#4'!K29, 'Run#5'!K29,'Run#6'!K29)</f>
+        <v>0.96610222076060592</v>
       </c>
       <c r="C2" s="2">
-        <f>AVERAGE('Run#1'!L29, 'Run#2'!L29, 'Run#3'!L29, 'Run#4'!L29, 'Run#5'!L29,'Run#6'!L29)</f>
-        <v>0.9795808211312087</v>
+        <f>AVERAGE('Run#0'!L29,'Run#1'!L29, 'Run#2'!L29, 'Run#3'!L29, 'Run#4'!L29, 'Run#5'!L29,'Run#6'!L29)</f>
+        <v>0.98249784668389317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>